<commit_message>
diseño de modulos en excel
</commit_message>
<xml_diff>
--- a/public/recursos/Diseño.xlsx
+++ b/public/recursos/Diseño.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asus\Avaluamos\Modelos_Avaluos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WWW\avaluamos\public\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300487EC-8C5D-43F4-8FAA-5B5AC116042D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F667E8-5AAE-4E91-B74E-F0ABE96DFFFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="251">
   <si>
     <t>HEADER</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>FOOTER</t>
-  </si>
-  <si>
-    <t>CONTENIDO MÓDULO</t>
   </si>
   <si>
     <t>id_avaluo</t>
@@ -774,19 +771,41 @@
     </r>
   </si>
   <si>
-    <t>TIEMPO</t>
-  </si>
-  <si>
     <t>VALOR HORA</t>
   </si>
   <si>
     <t>Permisos (por rol)</t>
+  </si>
+  <si>
+    <t>diario</t>
+  </si>
+  <si>
+    <t>valor hora</t>
+  </si>
+  <si>
+    <t>semana</t>
+  </si>
+  <si>
+    <t>mes</t>
+  </si>
+  <si>
+    <t>modulo</t>
+  </si>
+  <si>
+    <t>TIEMPO semanas</t>
+  </si>
+  <si>
+    <t>CONTENIDO MÓDULO
+incluye sopote 4 meses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$$-240A]\ #,##0"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1108,7 +1127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1203,24 +1222,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1230,33 +1288,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1275,50 +1330,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1600,10 +1637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E4" sqref="E4:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,189 +1649,289 @@
     <col min="2" max="2" width="46.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="46.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="80.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:9" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-    </row>
-    <row r="2" spans="1:5" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="70" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+    </row>
+    <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" s="42"/>
+      <c r="G2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="H2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42">
+        <f>SUM(C4:C12)</f>
+        <v>12</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+    </row>
+    <row r="4" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D2" s="70" t="s">
-        <v>244</v>
-      </c>
-      <c r="E2" s="70"/>
-    </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="C4" s="50">
+        <v>2</v>
+      </c>
+      <c r="D4" s="72">
+        <f>H9*5%</f>
+        <v>510000</v>
+      </c>
+      <c r="E4" s="76" t="s">
+        <v>250</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H4" s="68">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50"/>
+      <c r="B5" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
-      <c r="B4" s="29" t="s">
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="53"/>
+      <c r="G5" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H5" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="30"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="53"/>
+      <c r="G6" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H6" s="68">
+        <f>H5*H4</f>
+        <v>850000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="56" t="s">
         <v>236</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="40"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="40"/>
-    </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="s">
-        <v>237</v>
-      </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="40"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
-        <v>233</v>
-      </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="40"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="B7" s="57"/>
+      <c r="C7" s="36">
+        <v>2</v>
+      </c>
+      <c r="D7" s="73">
+        <f>H9*10%</f>
+        <v>1020000</v>
+      </c>
+      <c r="E7" s="53"/>
+      <c r="G7" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H7" s="68">
+        <f>H6*4</f>
+        <v>3400000</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="54" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8" s="55"/>
+      <c r="C8" s="37">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="D8" s="73">
+        <f>H9*10%</f>
+        <v>1020000</v>
+      </c>
+      <c r="E8" s="53"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="40"/>
-    </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
-      <c r="B9" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="40"/>
-    </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57" t="s">
+      <c r="C9" s="38">
+        <v>1</v>
+      </c>
+      <c r="D9" s="71">
+        <f>H9*60%</f>
+        <v>6120000</v>
+      </c>
+      <c r="E9" s="53"/>
+      <c r="H9" s="68">
+        <f>C3*H6</f>
+        <v>10200000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="52"/>
+      <c r="B10" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C10" s="38">
+        <v>3</v>
+      </c>
+      <c r="D10" s="70"/>
+      <c r="E10" s="53"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="58" t="s">
+        <v>238</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="C11" s="69">
+        <v>1.5</v>
+      </c>
+      <c r="D11" s="73">
+        <f>H9*7.5%</f>
+        <v>765000</v>
+      </c>
+      <c r="E11" s="53"/>
+      <c r="H11" s="68">
+        <f>H7*5</f>
+        <v>17000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="59"/>
+      <c r="B12" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="40"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="58"/>
-      <c r="B11" s="56" t="s">
-        <v>241</v>
-      </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="40"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="40"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="69">
+        <v>1.5</v>
+      </c>
+      <c r="D12" s="73">
+        <f>H9*7.5%</f>
+        <v>765000</v>
+      </c>
+      <c r="E12" s="53"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30"/>
       <c r="B13" s="31"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="40"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="41" t="s">
-        <v>242</v>
-      </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="40"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="48" t="s">
-        <v>238</v>
-      </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="40"/>
-    </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
-        <v>234</v>
-      </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="40"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="53"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="30"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="74">
+        <f>SUM(D4:D12)</f>
+        <v>10200000</v>
+      </c>
+      <c r="E14" s="53"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="60" t="s">
+        <v>241</v>
+      </c>
+      <c r="B15" s="61"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="53"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="46" t="s">
+        <v>237</v>
+      </c>
+      <c r="B16" s="47"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="74">
+        <f>D14*10%</f>
+        <v>1020000</v>
+      </c>
+      <c r="E16" s="53"/>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="75">
+        <f>D14-D16</f>
+        <v>9180000</v>
+      </c>
+      <c r="E17" s="53"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="40"/>
-    </row>
-    <row r="18" spans="1:5" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45" t="s">
+      <c r="B18" s="47"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="53"/>
+    </row>
+    <row r="19" spans="1:5" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="47"/>
-    </row>
-    <row r="19" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+    </row>
+    <row r="20" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A18:E18"/>
+  <mergeCells count="14">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="E4:E18"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E3:E17"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1820,65 +1957,65 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
+      <c r="A2" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
     </row>
     <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
-        <v>17</v>
-      </c>
       <c r="B4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="21"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="21"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="21"/>
@@ -1886,7 +2023,7 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="21"/>
@@ -1894,854 +2031,854 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="21"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
-        <v>15</v>
+      <c r="A11" s="62" t="s">
+        <v>14</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="21"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="21"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="21"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="21"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="21"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>28</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="21"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="21"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="21"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="21"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
+      <c r="A24" s="62"/>
       <c r="B24" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="21"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>35</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
+      <c r="A26" s="62"/>
       <c r="B26" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="21"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
+      <c r="A28" s="62"/>
       <c r="B28" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="21"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="21"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="21"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="21"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="21"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
+      <c r="A33" s="62"/>
       <c r="B33" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="21"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
+      <c r="A34" s="62"/>
       <c r="B34" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="21"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="50"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="21"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="50"/>
+      <c r="A36" s="62"/>
       <c r="B36" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="21"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="50"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="21"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="50"/>
+      <c r="A38" s="62"/>
       <c r="B38" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="21"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="50"/>
+      <c r="A39" s="62"/>
       <c r="B39" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="21"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="50"/>
+      <c r="A40" s="62"/>
       <c r="B40" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="21"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="22"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="52" t="s">
+      <c r="A42" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="20"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="53"/>
+      <c r="A43" s="65"/>
       <c r="B43" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="21"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="53"/>
+      <c r="A44" s="65"/>
       <c r="B44" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="21"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="53"/>
+      <c r="A45" s="65"/>
       <c r="B45" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="21"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="53"/>
+      <c r="A46" s="65"/>
       <c r="B46" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="21"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="53"/>
+      <c r="A47" s="65"/>
       <c r="B47" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="21"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="53"/>
+      <c r="A48" s="65"/>
       <c r="B48" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="21"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="53"/>
+      <c r="A49" s="65"/>
       <c r="B49" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="21"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="53"/>
+      <c r="A50" s="65"/>
       <c r="B50" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" s="9"/>
       <c r="D50" s="21"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="53"/>
+      <c r="A51" s="65"/>
       <c r="B51" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="21"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="53"/>
+      <c r="A52" s="65"/>
       <c r="B52" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="9" t="s">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="65"/>
+      <c r="B53" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D52" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="53"/>
-      <c r="B53" s="10" t="s">
+      <c r="C53" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="D53" s="21"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="65"/>
+      <c r="B54" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D53" s="21"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="53"/>
-      <c r="B54" s="10" t="s">
+      <c r="C54" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="D54" s="21"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="65"/>
+      <c r="B55" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D54" s="21"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="53"/>
-      <c r="B55" s="10" t="s">
+      <c r="C55" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55" s="21"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="65"/>
+      <c r="B56" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="21"/>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="66"/>
+      <c r="B57" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C55" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D55" s="21"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="53"/>
-      <c r="B56" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D56" s="21"/>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="54"/>
-      <c r="B57" s="12" t="s">
+      <c r="C57" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D57" s="23"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="23"/>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="52" t="s">
+      <c r="B58" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B58" s="8" t="s">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="65"/>
+      <c r="B59" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="65"/>
+      <c r="B60" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="65"/>
+      <c r="B61" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="65"/>
+      <c r="B62" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D62" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C58" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="53"/>
-      <c r="B59" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D59" s="21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="53"/>
-      <c r="B60" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D60" s="21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="53"/>
-      <c r="B61" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" s="21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="53"/>
-      <c r="B62" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D62" s="21" t="s">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="65"/>
+      <c r="B63" s="10" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="53"/>
-      <c r="B63" s="10" t="s">
+      <c r="C63" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="65"/>
+      <c r="B64" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C63" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D63" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="53"/>
-      <c r="B64" s="10" t="s">
+      <c r="C64" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D64" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="C64" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D64" s="21" t="s">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="65"/>
+      <c r="B65" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="53"/>
-      <c r="B65" s="10" t="s">
+      <c r="C65" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C65" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D65" s="21" t="s">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="65"/>
+      <c r="B66" s="10" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="53"/>
-      <c r="B66" s="10" t="s">
+      <c r="C66" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D66" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C66" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D66" s="21" t="s">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="65"/>
+      <c r="B67" s="10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="53"/>
-      <c r="B67" s="10" t="s">
+      <c r="C67" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C67" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D67" s="21" t="s">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="65"/>
+      <c r="B68" s="10" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="53"/>
-      <c r="B68" s="10" t="s">
+      <c r="C68" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D68" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C68" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D68" s="21" t="s">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="65"/>
+      <c r="B69" s="10" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="53"/>
-      <c r="B69" s="10" t="s">
+      <c r="C69" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D69" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C69" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D69" s="21" t="s">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="65"/>
+      <c r="B70" s="10" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="53"/>
-      <c r="B70" s="10" t="s">
+      <c r="C70" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D70" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C70" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D70" s="21" t="s">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="65"/>
+      <c r="B71" s="10" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="53"/>
-      <c r="B71" s="10" t="s">
+      <c r="C71" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D71" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C71" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D71" s="21" t="s">
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="65"/>
+      <c r="B72" s="10" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="53"/>
-      <c r="B72" s="10" t="s">
+      <c r="C72" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D72" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C72" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D72" s="21" t="s">
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="65"/>
+      <c r="B73" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D73" s="21" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="53"/>
-      <c r="B73" s="10" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="65"/>
+      <c r="B74" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C73" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D73" s="21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="53"/>
-      <c r="B74" s="10" t="s">
+      <c r="C74" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D74" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C74" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D74" s="21" t="s">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="65"/>
+      <c r="B75" s="10" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="53"/>
-      <c r="B75" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="C75" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D75" s="21">
         <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="53"/>
+      <c r="A76" s="65"/>
       <c r="B76" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D76" s="21">
         <v>2012</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="53"/>
+      <c r="A77" s="65"/>
       <c r="B77" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D77" s="21">
         <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="53"/>
+      <c r="A78" s="65"/>
       <c r="B78" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D78" s="25">
         <v>8.48E-2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="53"/>
+      <c r="A79" s="65"/>
       <c r="B79" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D79" s="21">
         <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="54"/>
+      <c r="A80" s="66"/>
       <c r="B80" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D80" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="64" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="52" t="s">
+      <c r="B81" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="C81" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="65"/>
+      <c r="B82" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C81" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D81" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="53"/>
-      <c r="B82" s="10" t="s">
+      <c r="C82" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="65"/>
+      <c r="B83" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C82" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D82" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="53"/>
-      <c r="B83" s="10" t="s">
+      <c r="C83" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D83" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="65"/>
+      <c r="B84" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C83" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D83" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="53"/>
-      <c r="B84" s="10" t="s">
+      <c r="C84" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D84" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="65"/>
+      <c r="B85" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C84" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D84" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="53"/>
-      <c r="B85" s="10" t="s">
+      <c r="C85" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D85" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="65"/>
+      <c r="B86" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C85" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D85" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="53"/>
-      <c r="B86" s="10" t="s">
+      <c r="C86" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D86" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="65"/>
+      <c r="B87" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C86" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D86" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="53"/>
-      <c r="B87" s="10" t="s">
+      <c r="C87" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D87" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="65"/>
+      <c r="B88" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C87" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D87" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="53"/>
-      <c r="B88" s="10" t="s">
+      <c r="C88" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="65"/>
+      <c r="B89" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C88" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D88" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="53"/>
-      <c r="B89" s="10" t="s">
+      <c r="C89" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="65"/>
+      <c r="B90" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C89" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D89" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="53"/>
-      <c r="B90" s="10" t="s">
+      <c r="C90" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D90" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="65"/>
+      <c r="B91" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C90" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="53"/>
-      <c r="B91" s="10" t="s">
+      <c r="C91" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D91" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="65"/>
+      <c r="B92" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="C91" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D91" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="53"/>
-      <c r="B92" s="10" t="s">
+      <c r="C92" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D92" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="66"/>
+      <c r="B93" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C93" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D93" s="23" t="s">
         <v>127</v>
-      </c>
-      <c r="C92" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D92" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="54"/>
-      <c r="B93" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C93" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D93" s="23" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B94" s="13"/>
       <c r="C94" s="17"/>
@@ -5219,27 +5356,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>134</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="C2" s="28" t="s">
         <v>137</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>138</v>
       </c>
       <c r="D2" s="27">
         <v>2</v>
@@ -5247,13 +5384,13 @@
     </row>
     <row r="3" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="28" t="s">
         <v>140</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>141</v>
       </c>
       <c r="D3" s="27">
         <v>125</v>
@@ -5261,13 +5398,13 @@
     </row>
     <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>142</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>143</v>
       </c>
       <c r="D4" s="27">
         <v>7</v>
@@ -5275,13 +5412,13 @@
     </row>
     <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="C5" s="28" t="s">
         <v>145</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>146</v>
       </c>
       <c r="D5" s="27">
         <v>23</v>
@@ -5289,27 +5426,27 @@
     </row>
     <row r="6" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="28" t="s">
+      <c r="D6" s="27" t="s">
         <v>148</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="C7" s="28" t="s">
         <v>151</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>152</v>
       </c>
       <c r="D7" s="27">
         <v>45</v>
@@ -5317,13 +5454,13 @@
     </row>
     <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="C8" s="28" t="s">
         <v>154</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>155</v>
       </c>
       <c r="D8" s="27">
         <v>123</v>
@@ -5331,13 +5468,13 @@
     </row>
     <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="C9" s="28" t="s">
         <v>157</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>158</v>
       </c>
       <c r="D9" s="27">
         <v>27</v>
@@ -5345,13 +5482,13 @@
     </row>
     <row r="10" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="C10" s="28" t="s">
         <v>160</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>161</v>
       </c>
       <c r="D10" s="27">
         <v>16</v>
@@ -5359,13 +5496,13 @@
     </row>
     <row r="11" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="C11" s="28" t="s">
         <v>163</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>164</v>
       </c>
       <c r="D11" s="27">
         <v>19</v>
@@ -5373,13 +5510,13 @@
     </row>
     <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="C12" s="28" t="s">
         <v>166</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>167</v>
       </c>
       <c r="D12" s="27">
         <v>41</v>
@@ -5387,13 +5524,13 @@
     </row>
     <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="C13" s="28" t="s">
         <v>169</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>170</v>
       </c>
       <c r="D13" s="27">
         <v>25</v>
@@ -5401,13 +5538,13 @@
     </row>
     <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="C14" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>173</v>
       </c>
       <c r="D14" s="27">
         <v>31</v>
@@ -5415,13 +5552,13 @@
     </row>
     <row r="15" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="C15" s="28" t="s">
         <v>175</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>176</v>
       </c>
       <c r="D15" s="27">
         <v>30</v>
@@ -5429,13 +5566,13 @@
     </row>
     <row r="16" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>177</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>178</v>
       </c>
       <c r="D16" s="27">
         <v>116</v>
@@ -5443,13 +5580,13 @@
     </row>
     <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="C17" s="28" t="s">
         <v>180</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>181</v>
       </c>
       <c r="D17" s="27">
         <v>1</v>
@@ -5457,13 +5594,13 @@
     </row>
     <row r="18" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="C18" s="28" t="s">
         <v>183</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>184</v>
       </c>
       <c r="D18" s="27">
         <v>4</v>
@@ -5471,13 +5608,13 @@
     </row>
     <row r="19" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="C19" s="28" t="s">
         <v>186</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>187</v>
       </c>
       <c r="D19" s="27">
         <v>37</v>
@@ -5485,13 +5622,13 @@
     </row>
     <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="C20" s="28" t="s">
         <v>189</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>190</v>
       </c>
       <c r="D20" s="27">
         <v>15</v>
@@ -5499,13 +5636,13 @@
     </row>
     <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="C21" s="28" t="s">
         <v>192</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>193</v>
       </c>
       <c r="D21" s="27">
         <v>30</v>
@@ -5513,13 +5650,13 @@
     </row>
     <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="B22" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="C22" s="28" t="s">
         <v>195</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>196</v>
       </c>
       <c r="D22" s="27">
         <v>29</v>
@@ -5527,13 +5664,13 @@
     </row>
     <row r="23" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="C23" s="28" t="s">
         <v>198</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>199</v>
       </c>
       <c r="D23" s="27">
         <v>64</v>
@@ -5541,13 +5678,13 @@
     </row>
     <row r="24" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="C24" s="28" t="s">
         <v>201</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>202</v>
       </c>
       <c r="D24" s="27">
         <v>40</v>
@@ -5555,13 +5692,13 @@
     </row>
     <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="C25" s="28" t="s">
         <v>204</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>205</v>
       </c>
       <c r="D25" s="27">
         <v>13</v>
@@ -5569,13 +5706,13 @@
     </row>
     <row r="26" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="B26" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="C26" s="28" t="s">
         <v>207</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>208</v>
       </c>
       <c r="D26" s="27">
         <v>12</v>
@@ -5583,13 +5720,13 @@
     </row>
     <row r="27" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="B27" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="C27" s="28" t="s">
         <v>210</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>211</v>
       </c>
       <c r="D27" s="27">
         <v>14</v>
@@ -5597,10 +5734,10 @@
     </row>
     <row r="28" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B28" s="27" t="s">
         <v>212</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>213</v>
       </c>
       <c r="C28" s="28">
         <v>52</v>
@@ -5611,13 +5748,13 @@
     </row>
     <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B29" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="C29" s="28" t="s">
         <v>215</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>216</v>
       </c>
       <c r="D29" s="27">
         <v>87</v>
@@ -5625,13 +5762,13 @@
     </row>
     <row r="30" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="B30" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="C30" s="28" t="s">
         <v>218</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>219</v>
       </c>
       <c r="D30" s="27">
         <v>26</v>
@@ -5639,13 +5776,13 @@
     </row>
     <row r="31" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="B31" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="C31" s="28" t="s">
         <v>221</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>222</v>
       </c>
       <c r="D31" s="27">
         <v>47</v>
@@ -5653,13 +5790,13 @@
     </row>
     <row r="32" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="C32" s="28" t="s">
         <v>224</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>225</v>
       </c>
       <c r="D32" s="27">
         <v>42</v>
@@ -5667,13 +5804,13 @@
     </row>
     <row r="33" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="B33" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="C33" s="28" t="s">
         <v>227</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>228</v>
       </c>
       <c r="D33" s="27">
         <v>3</v>
@@ -5681,13 +5818,13 @@
     </row>
     <row r="34" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="B34" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="C34" s="28" t="s">
         <v>230</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>231</v>
       </c>
       <c r="D34" s="27">
         <v>4</v>
@@ -5717,27 +5854,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>134</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="C2" s="28" t="s">
         <v>137</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>138</v>
       </c>
       <c r="D2" s="27">
         <v>2</v>
@@ -5745,13 +5882,13 @@
     </row>
     <row r="3" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="28" t="s">
         <v>140</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>141</v>
       </c>
       <c r="D3" s="27">
         <v>125</v>
@@ -5759,13 +5896,13 @@
     </row>
     <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>142</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>143</v>
       </c>
       <c r="D4" s="27">
         <v>7</v>
@@ -5773,13 +5910,13 @@
     </row>
     <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="C5" s="28" t="s">
         <v>145</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>146</v>
       </c>
       <c r="D5" s="27">
         <v>23</v>
@@ -5787,27 +5924,27 @@
     </row>
     <row r="6" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="28" t="s">
+      <c r="D6" s="27" t="s">
         <v>148</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="C7" s="28" t="s">
         <v>151</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>152</v>
       </c>
       <c r="D7" s="27">
         <v>45</v>
@@ -5815,13 +5952,13 @@
     </row>
     <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="C8" s="28" t="s">
         <v>154</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>155</v>
       </c>
       <c r="D8" s="27">
         <v>123</v>
@@ -5829,13 +5966,13 @@
     </row>
     <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="C9" s="28" t="s">
         <v>157</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>158</v>
       </c>
       <c r="D9" s="27">
         <v>27</v>
@@ -5843,13 +5980,13 @@
     </row>
     <row r="10" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="C10" s="28" t="s">
         <v>160</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>161</v>
       </c>
       <c r="D10" s="27">
         <v>16</v>
@@ -5857,13 +5994,13 @@
     </row>
     <row r="11" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="C11" s="28" t="s">
         <v>163</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>164</v>
       </c>
       <c r="D11" s="27">
         <v>19</v>
@@ -5871,13 +6008,13 @@
     </row>
     <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="C12" s="28" t="s">
         <v>166</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>167</v>
       </c>
       <c r="D12" s="27">
         <v>41</v>
@@ -5885,13 +6022,13 @@
     </row>
     <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="C13" s="28" t="s">
         <v>169</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>170</v>
       </c>
       <c r="D13" s="27">
         <v>25</v>
@@ -5899,13 +6036,13 @@
     </row>
     <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="C14" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>173</v>
       </c>
       <c r="D14" s="27">
         <v>31</v>
@@ -5913,13 +6050,13 @@
     </row>
     <row r="15" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="C15" s="28" t="s">
         <v>175</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>176</v>
       </c>
       <c r="D15" s="27">
         <v>30</v>
@@ -5927,13 +6064,13 @@
     </row>
     <row r="16" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>177</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>178</v>
       </c>
       <c r="D16" s="27">
         <v>116</v>
@@ -5941,13 +6078,13 @@
     </row>
     <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="C17" s="28" t="s">
         <v>180</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>181</v>
       </c>
       <c r="D17" s="27">
         <v>1</v>
@@ -5955,13 +6092,13 @@
     </row>
     <row r="18" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="C18" s="28" t="s">
         <v>183</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>184</v>
       </c>
       <c r="D18" s="27">
         <v>4</v>
@@ -5969,13 +6106,13 @@
     </row>
     <row r="19" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="C19" s="28" t="s">
         <v>186</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>187</v>
       </c>
       <c r="D19" s="27">
         <v>37</v>
@@ -5983,13 +6120,13 @@
     </row>
     <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="C20" s="28" t="s">
         <v>189</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>190</v>
       </c>
       <c r="D20" s="27">
         <v>15</v>
@@ -5997,13 +6134,13 @@
     </row>
     <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="C21" s="28" t="s">
         <v>192</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>193</v>
       </c>
       <c r="D21" s="27">
         <v>30</v>
@@ -6011,13 +6148,13 @@
     </row>
     <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="B22" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="C22" s="28" t="s">
         <v>195</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>196</v>
       </c>
       <c r="D22" s="27">
         <v>29</v>
@@ -6025,13 +6162,13 @@
     </row>
     <row r="23" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="C23" s="28" t="s">
         <v>198</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>199</v>
       </c>
       <c r="D23" s="27">
         <v>64</v>
@@ -6039,13 +6176,13 @@
     </row>
     <row r="24" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="C24" s="28" t="s">
         <v>201</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>202</v>
       </c>
       <c r="D24" s="27">
         <v>40</v>
@@ -6053,13 +6190,13 @@
     </row>
     <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="C25" s="28" t="s">
         <v>204</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>205</v>
       </c>
       <c r="D25" s="27">
         <v>13</v>
@@ -6067,13 +6204,13 @@
     </row>
     <row r="26" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="B26" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="C26" s="28" t="s">
         <v>207</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>208</v>
       </c>
       <c r="D26" s="27">
         <v>12</v>
@@ -6081,13 +6218,13 @@
     </row>
     <row r="27" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="B27" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="C27" s="28" t="s">
         <v>210</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>211</v>
       </c>
       <c r="D27" s="27">
         <v>14</v>
@@ -6095,10 +6232,10 @@
     </row>
     <row r="28" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B28" s="27" t="s">
         <v>212</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>213</v>
       </c>
       <c r="C28" s="28">
         <v>52</v>
@@ -6109,13 +6246,13 @@
     </row>
     <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B29" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="C29" s="28" t="s">
         <v>215</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>216</v>
       </c>
       <c r="D29" s="27">
         <v>87</v>
@@ -6123,13 +6260,13 @@
     </row>
     <row r="30" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="B30" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="C30" s="28" t="s">
         <v>218</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>219</v>
       </c>
       <c r="D30" s="27">
         <v>26</v>
@@ -6137,13 +6274,13 @@
     </row>
     <row r="31" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="B31" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="C31" s="28" t="s">
         <v>221</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>222</v>
       </c>
       <c r="D31" s="27">
         <v>47</v>
@@ -6151,13 +6288,13 @@
     </row>
     <row r="32" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="C32" s="28" t="s">
         <v>224</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>225</v>
       </c>
       <c r="D32" s="27">
         <v>42</v>
@@ -6165,13 +6302,13 @@
     </row>
     <row r="33" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="B33" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="C33" s="28" t="s">
         <v>227</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>228</v>
       </c>
       <c r="D33" s="27">
         <v>3</v>
@@ -6179,13 +6316,13 @@
     </row>
     <row r="34" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="B34" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="C34" s="28" t="s">
         <v>230</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>231</v>
       </c>
       <c r="D34" s="27">
         <v>4</v>

</xml_diff>

<commit_message>
Ajustes presupuesto para William
</commit_message>
<xml_diff>
--- a/public/recursos/Diseño.xlsx
+++ b/public/recursos/Diseño.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WWW\avaluamos\public\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F667E8-5AAE-4E91-B74E-F0ABE96DFFFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DA1E0E-C556-4ED2-9F88-74500BBE426F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diseño" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Dptos" sheetId="3" r:id="rId3"/>
     <sheet name="Ciudades" sheetId="4" r:id="rId4"/>
     <sheet name="Paises" sheetId="5" r:id="rId5"/>
+    <sheet name="Diseño (2)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="265">
   <si>
     <t>HEADER</t>
   </si>
@@ -798,6 +799,52 @@
     <t>CONTENIDO MÓDULO
 incluye sopote 4 meses</t>
   </si>
+  <si>
+    <t>MÓDULOS</t>
+  </si>
+  <si>
+    <t>VALO MÓDULO</t>
+  </si>
+  <si>
+    <t>HORAS SEMANALES</t>
+  </si>
+  <si>
+    <t>VALOR SEMANA</t>
+  </si>
+  <si>
+    <t>CANTIDAD SEMANAS</t>
+  </si>
+  <si>
+    <t>VALOR TOTAL</t>
+  </si>
+  <si>
+    <t>TIEMPO EN SEMANAS</t>
+  </si>
+  <si>
+    <t>SUB-MÓDULOS</t>
+  </si>
+  <si>
+    <t>Crear/ Editar/Leer</t>
+  </si>
+  <si>
+    <t>PRESUPUESTO APLICACIÓN WEB "AVALUAMOS"</t>
+  </si>
+  <si>
+    <t>CANTIDAD
+ MÓDULOS</t>
+  </si>
+  <si>
+    <t>OBSERVACIONES</t>
+  </si>
+  <si>
+    <t>HORAS DIARIAS
+(Lunes a Viernes)</t>
+  </si>
+  <si>
+    <t>1. Incluye soporte por 4 meses
+2. El tiempo adicional es asumido por el desarrollador
+3. Las solicitudes adicionales serán negociadas y asumidas con valor adicional</t>
+  </si>
 </sst>
 </file>
 
@@ -806,7 +853,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-240A]\ #,##0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -850,8 +897,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -906,8 +984,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1123,11 +1213,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1255,6 +1376,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1286,6 +1422,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1312,6 +1451,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1330,32 +1478,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1639,7 +1829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="E4" sqref="E4:E18"/>
     </sheetView>
   </sheetViews>
@@ -1656,13 +1846,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41"/>
@@ -1692,37 +1882,37 @@
       <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="54" t="s">
         <v>234</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C4" s="50">
+      <c r="C4" s="55">
         <v>2</v>
       </c>
-      <c r="D4" s="72">
+      <c r="D4" s="68">
         <f>H9*5%</f>
         <v>510000</v>
       </c>
-      <c r="E4" s="76" t="s">
+      <c r="E4" s="58" t="s">
         <v>250</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="H4" s="68">
+      <c r="H4" s="43">
         <v>17000</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="53"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="59"/>
       <c r="G5" s="1" t="s">
         <v>246</v>
       </c>
@@ -1735,32 +1925,32 @@
       <c r="B6" s="31"/>
       <c r="C6" s="35"/>
       <c r="D6" s="35"/>
-      <c r="E6" s="53"/>
+      <c r="E6" s="59"/>
       <c r="G6" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="H6" s="68">
+      <c r="H6" s="43">
         <f>H5*H4</f>
         <v>850000</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="B7" s="57"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="36">
         <v>2</v>
       </c>
-      <c r="D7" s="73">
+      <c r="D7" s="45">
         <f>H9*10%</f>
         <v>1020000</v>
       </c>
-      <c r="E7" s="53"/>
+      <c r="E7" s="59"/>
       <c r="G7" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="H7" s="68">
+      <c r="H7" s="43">
         <f>H6*4</f>
         <v>3400000</v>
       </c>
@@ -1769,21 +1959,21 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="60" t="s">
         <v>232</v>
       </c>
-      <c r="B8" s="55"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="37">
         <v>1</v>
       </c>
-      <c r="D8" s="73">
+      <c r="D8" s="45">
         <f>H9*10%</f>
         <v>1020000</v>
       </c>
-      <c r="E8" s="53"/>
+      <c r="E8" s="59"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="56" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1792,18 +1982,18 @@
       <c r="C9" s="38">
         <v>1</v>
       </c>
-      <c r="D9" s="71">
+      <c r="D9" s="69">
         <f>H9*60%</f>
         <v>6120000</v>
       </c>
-      <c r="E9" s="53"/>
-      <c r="H9" s="68">
+      <c r="E9" s="59"/>
+      <c r="H9" s="43">
         <f>C3*H6</f>
         <v>10200000</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="4" t="s">
         <v>231</v>
       </c>
@@ -1811,79 +2001,79 @@
         <v>3</v>
       </c>
       <c r="D10" s="70"/>
-      <c r="E10" s="53"/>
+      <c r="E10" s="59"/>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="64" t="s">
         <v>238</v>
       </c>
       <c r="B11" s="34" t="s">
         <v>239</v>
       </c>
-      <c r="C11" s="69">
+      <c r="C11" s="44">
         <v>1.5</v>
       </c>
-      <c r="D11" s="73">
+      <c r="D11" s="45">
         <f>H9*7.5%</f>
         <v>765000</v>
       </c>
-      <c r="E11" s="53"/>
-      <c r="H11" s="68">
+      <c r="E11" s="59"/>
+      <c r="H11" s="43">
         <f>H7*5</f>
         <v>17000000</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="59"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="C12" s="69">
+      <c r="C12" s="44">
         <v>1.5</v>
       </c>
-      <c r="D12" s="73">
+      <c r="D12" s="45">
         <f>H9*7.5%</f>
         <v>765000</v>
       </c>
-      <c r="E12" s="53"/>
+      <c r="E12" s="59"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30"/>
       <c r="B13" s="31"/>
       <c r="C13" s="35"/>
       <c r="D13" s="35"/>
-      <c r="E13" s="53"/>
+      <c r="E13" s="59"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30"/>
       <c r="B14" s="31"/>
       <c r="C14" s="35"/>
-      <c r="D14" s="74">
+      <c r="D14" s="46">
         <f>SUM(D4:D12)</f>
         <v>10200000</v>
       </c>
-      <c r="E14" s="53"/>
+      <c r="E14" s="59"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="66" t="s">
         <v>241</v>
       </c>
-      <c r="B15" s="61"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
-      <c r="E15" s="53"/>
+      <c r="E15" s="59"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="51" t="s">
         <v>237</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="35"/>
-      <c r="D16" s="74">
+      <c r="D16" s="46">
         <f>D14*10%</f>
         <v>1020000</v>
       </c>
-      <c r="E16" s="53"/>
+      <c r="E16" s="59"/>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
@@ -1891,29 +2081,29 @@
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="40"/>
-      <c r="D17" s="75">
+      <c r="D17" s="47">
         <f>D14-D16</f>
         <v>9180000</v>
       </c>
-      <c r="E17" s="53"/>
+      <c r="E17" s="59"/>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="35"/>
       <c r="D18" s="35"/>
-      <c r="E18" s="53"/>
+      <c r="E18" s="59"/>
     </row>
     <row r="19" spans="1:5" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="50"/>
     </row>
     <row r="20" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -1957,12 +2147,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
     </row>
     <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -1979,7 +2169,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="76" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1989,7 +2179,7 @@
       <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
+      <c r="A5" s="71"/>
       <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
@@ -1997,7 +2187,7 @@
       <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
+      <c r="A6" s="71"/>
       <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
@@ -2005,7 +2195,7 @@
       <c r="D6" s="21"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
@@ -2013,7 +2203,7 @@
       <c r="D7" s="21"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
@@ -2037,7 +2227,7 @@
       <c r="D10" s="21"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="71" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -2047,7 +2237,7 @@
       <c r="D11" s="21"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
+      <c r="A12" s="71"/>
       <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
@@ -2055,7 +2245,7 @@
       <c r="D12" s="21"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
+      <c r="A13" s="71"/>
       <c r="B13" s="10" t="s">
         <v>18</v>
       </c>
@@ -2063,7 +2253,7 @@
       <c r="D13" s="21"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="71" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -2073,7 +2263,7 @@
       <c r="D14" s="21"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
+      <c r="A15" s="71"/>
       <c r="B15" s="10" t="s">
         <v>21</v>
       </c>
@@ -2081,7 +2271,7 @@
       <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="62"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="10" t="s">
         <v>22</v>
       </c>
@@ -2089,7 +2279,7 @@
       <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="62" t="s">
+      <c r="A17" s="71" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -2099,7 +2289,7 @@
       <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
+      <c r="A18" s="71"/>
       <c r="B18" s="10" t="s">
         <v>25</v>
       </c>
@@ -2107,7 +2297,7 @@
       <c r="D18" s="21"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="62" t="s">
+      <c r="A19" s="71" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -2117,7 +2307,7 @@
       <c r="D19" s="21"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
+      <c r="A20" s="71"/>
       <c r="B20" s="10" t="s">
         <v>28</v>
       </c>
@@ -2125,7 +2315,7 @@
       <c r="D20" s="21"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
+      <c r="A21" s="71"/>
       <c r="B21" s="10" t="s">
         <v>29</v>
       </c>
@@ -2133,7 +2323,7 @@
       <c r="D21" s="21"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="62"/>
+      <c r="A22" s="71"/>
       <c r="B22" s="10" t="s">
         <v>30</v>
       </c>
@@ -2141,7 +2331,7 @@
       <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
+      <c r="A23" s="71"/>
       <c r="B23" s="10" t="s">
         <v>32</v>
       </c>
@@ -2149,7 +2339,7 @@
       <c r="D23" s="21"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="62"/>
+      <c r="A24" s="71"/>
       <c r="B24" s="10" t="s">
         <v>31</v>
       </c>
@@ -2157,7 +2347,7 @@
       <c r="D24" s="21"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="62" t="s">
+      <c r="A25" s="71" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -2167,7 +2357,7 @@
       <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
+      <c r="A26" s="71"/>
       <c r="B26" s="10" t="s">
         <v>35</v>
       </c>
@@ -2175,7 +2365,7 @@
       <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="62"/>
+      <c r="A27" s="71"/>
       <c r="B27" s="10" t="s">
         <v>36</v>
       </c>
@@ -2183,7 +2373,7 @@
       <c r="D27" s="21"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="62"/>
+      <c r="A28" s="71"/>
       <c r="B28" s="10" t="s">
         <v>37</v>
       </c>
@@ -2191,7 +2381,7 @@
       <c r="D28" s="21"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
+      <c r="A29" s="71"/>
       <c r="B29" s="10" t="s">
         <v>39</v>
       </c>
@@ -2199,7 +2389,7 @@
       <c r="D29" s="21"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
+      <c r="A30" s="71"/>
       <c r="B30" s="10" t="s">
         <v>38</v>
       </c>
@@ -2207,7 +2397,7 @@
       <c r="D30" s="21"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
+      <c r="A31" s="71"/>
       <c r="B31" s="10" t="s">
         <v>40</v>
       </c>
@@ -2215,7 +2405,7 @@
       <c r="D31" s="21"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
+      <c r="A32" s="71"/>
       <c r="B32" s="10" t="s">
         <v>41</v>
       </c>
@@ -2223,7 +2413,7 @@
       <c r="D32" s="21"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
+      <c r="A33" s="71"/>
       <c r="B33" s="10" t="s">
         <v>42</v>
       </c>
@@ -2231,7 +2421,7 @@
       <c r="D33" s="21"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="62"/>
+      <c r="A34" s="71"/>
       <c r="B34" s="10" t="s">
         <v>43</v>
       </c>
@@ -2239,7 +2429,7 @@
       <c r="D34" s="21"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="62"/>
+      <c r="A35" s="71"/>
       <c r="B35" s="10" t="s">
         <v>44</v>
       </c>
@@ -2247,7 +2437,7 @@
       <c r="D35" s="21"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="62"/>
+      <c r="A36" s="71"/>
       <c r="B36" s="10" t="s">
         <v>45</v>
       </c>
@@ -2255,7 +2445,7 @@
       <c r="D36" s="21"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="62"/>
+      <c r="A37" s="71"/>
       <c r="B37" s="10" t="s">
         <v>46</v>
       </c>
@@ -2263,7 +2453,7 @@
       <c r="D37" s="21"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="62"/>
+      <c r="A38" s="71"/>
       <c r="B38" s="10" t="s">
         <v>47</v>
       </c>
@@ -2271,7 +2461,7 @@
       <c r="D38" s="21"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="62"/>
+      <c r="A39" s="71"/>
       <c r="B39" s="10" t="s">
         <v>48</v>
       </c>
@@ -2279,7 +2469,7 @@
       <c r="D39" s="21"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="62"/>
+      <c r="A40" s="71"/>
       <c r="B40" s="10" t="s">
         <v>49</v>
       </c>
@@ -2297,7 +2487,7 @@
       <c r="D41" s="22"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="64" t="s">
+      <c r="A42" s="73" t="s">
         <v>52</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -2307,7 +2497,7 @@
       <c r="D42" s="20"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="65"/>
+      <c r="A43" s="74"/>
       <c r="B43" s="10" t="s">
         <v>54</v>
       </c>
@@ -2315,7 +2505,7 @@
       <c r="D43" s="21"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="65"/>
+      <c r="A44" s="74"/>
       <c r="B44" s="10" t="s">
         <v>55</v>
       </c>
@@ -2323,7 +2513,7 @@
       <c r="D44" s="21"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="65"/>
+      <c r="A45" s="74"/>
       <c r="B45" s="10" t="s">
         <v>56</v>
       </c>
@@ -2331,7 +2521,7 @@
       <c r="D45" s="21"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="65"/>
+      <c r="A46" s="74"/>
       <c r="B46" s="10" t="s">
         <v>57</v>
       </c>
@@ -2339,7 +2529,7 @@
       <c r="D46" s="21"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="65"/>
+      <c r="A47" s="74"/>
       <c r="B47" s="10" t="s">
         <v>58</v>
       </c>
@@ -2347,7 +2537,7 @@
       <c r="D47" s="21"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="65"/>
+      <c r="A48" s="74"/>
       <c r="B48" s="10" t="s">
         <v>59</v>
       </c>
@@ -2355,7 +2545,7 @@
       <c r="D48" s="21"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="65"/>
+      <c r="A49" s="74"/>
       <c r="B49" s="10" t="s">
         <v>60</v>
       </c>
@@ -2363,7 +2553,7 @@
       <c r="D49" s="21"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="65"/>
+      <c r="A50" s="74"/>
       <c r="B50" s="10" t="s">
         <v>61</v>
       </c>
@@ -2371,7 +2561,7 @@
       <c r="D50" s="21"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="65"/>
+      <c r="A51" s="74"/>
       <c r="B51" s="10" t="s">
         <v>62</v>
       </c>
@@ -2379,7 +2569,7 @@
       <c r="D51" s="21"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="65"/>
+      <c r="A52" s="74"/>
       <c r="B52" s="10" t="s">
         <v>63</v>
       </c>
@@ -2391,7 +2581,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="65"/>
+      <c r="A53" s="74"/>
       <c r="B53" s="10" t="s">
         <v>68</v>
       </c>
@@ -2401,7 +2591,7 @@
       <c r="D53" s="21"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="65"/>
+      <c r="A54" s="74"/>
       <c r="B54" s="10" t="s">
         <v>70</v>
       </c>
@@ -2411,7 +2601,7 @@
       <c r="D54" s="21"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="65"/>
+      <c r="A55" s="74"/>
       <c r="B55" s="10" t="s">
         <v>72</v>
       </c>
@@ -2421,7 +2611,7 @@
       <c r="D55" s="21"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="65"/>
+      <c r="A56" s="74"/>
       <c r="B56" s="10" t="s">
         <v>49</v>
       </c>
@@ -2431,7 +2621,7 @@
       <c r="D56" s="21"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="66"/>
+      <c r="A57" s="75"/>
       <c r="B57" s="12" t="s">
         <v>73</v>
       </c>
@@ -2441,7 +2631,7 @@
       <c r="D57" s="23"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="64" t="s">
+      <c r="A58" s="73" t="s">
         <v>74</v>
       </c>
       <c r="B58" s="8" t="s">
@@ -2455,7 +2645,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="65"/>
+      <c r="A59" s="74"/>
       <c r="B59" s="10" t="s">
         <v>76</v>
       </c>
@@ -2467,7 +2657,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="65"/>
+      <c r="A60" s="74"/>
       <c r="B60" s="10" t="s">
         <v>79</v>
       </c>
@@ -2479,7 +2669,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="65"/>
+      <c r="A61" s="74"/>
       <c r="B61" s="10" t="s">
         <v>81</v>
       </c>
@@ -2491,7 +2681,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="65"/>
+      <c r="A62" s="74"/>
       <c r="B62" s="10" t="s">
         <v>82</v>
       </c>
@@ -2503,7 +2693,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="65"/>
+      <c r="A63" s="74"/>
       <c r="B63" s="10" t="s">
         <v>85</v>
       </c>
@@ -2515,7 +2705,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="65"/>
+      <c r="A64" s="74"/>
       <c r="B64" s="10" t="s">
         <v>86</v>
       </c>
@@ -2527,7 +2717,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="65"/>
+      <c r="A65" s="74"/>
       <c r="B65" s="10" t="s">
         <v>88</v>
       </c>
@@ -2539,7 +2729,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="65"/>
+      <c r="A66" s="74"/>
       <c r="B66" s="10" t="s">
         <v>90</v>
       </c>
@@ -2551,7 +2741,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="65"/>
+      <c r="A67" s="74"/>
       <c r="B67" s="10" t="s">
         <v>92</v>
       </c>
@@ -2563,7 +2753,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="65"/>
+      <c r="A68" s="74"/>
       <c r="B68" s="10" t="s">
         <v>94</v>
       </c>
@@ -2575,7 +2765,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="65"/>
+      <c r="A69" s="74"/>
       <c r="B69" s="10" t="s">
         <v>96</v>
       </c>
@@ -2587,7 +2777,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="65"/>
+      <c r="A70" s="74"/>
       <c r="B70" s="10" t="s">
         <v>98</v>
       </c>
@@ -2599,7 +2789,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="65"/>
+      <c r="A71" s="74"/>
       <c r="B71" s="10" t="s">
         <v>100</v>
       </c>
@@ -2611,7 +2801,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="65"/>
+      <c r="A72" s="74"/>
       <c r="B72" s="10" t="s">
         <v>102</v>
       </c>
@@ -2623,7 +2813,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="65"/>
+      <c r="A73" s="74"/>
       <c r="B73" s="10" t="s">
         <v>105</v>
       </c>
@@ -2635,7 +2825,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="65"/>
+      <c r="A74" s="74"/>
       <c r="B74" s="10" t="s">
         <v>106</v>
       </c>
@@ -2647,7 +2837,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="65"/>
+      <c r="A75" s="74"/>
       <c r="B75" s="10" t="s">
         <v>108</v>
       </c>
@@ -2659,7 +2849,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="65"/>
+      <c r="A76" s="74"/>
       <c r="B76" s="10" t="s">
         <v>109</v>
       </c>
@@ -2671,7 +2861,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="65"/>
+      <c r="A77" s="74"/>
       <c r="B77" s="10" t="s">
         <v>110</v>
       </c>
@@ -2683,7 +2873,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="65"/>
+      <c r="A78" s="74"/>
       <c r="B78" s="10" t="s">
         <v>111</v>
       </c>
@@ -2695,7 +2885,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="65"/>
+      <c r="A79" s="74"/>
       <c r="B79" s="10" t="s">
         <v>112</v>
       </c>
@@ -2707,7 +2897,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="66"/>
+      <c r="A80" s="75"/>
       <c r="B80" s="12" t="s">
         <v>49</v>
       </c>
@@ -2719,7 +2909,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="64" t="s">
+      <c r="A81" s="73" t="s">
         <v>114</v>
       </c>
       <c r="B81" s="8" t="s">
@@ -2733,7 +2923,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="65"/>
+      <c r="A82" s="74"/>
       <c r="B82" s="10" t="s">
         <v>116</v>
       </c>
@@ -2745,7 +2935,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="65"/>
+      <c r="A83" s="74"/>
       <c r="B83" s="10" t="s">
         <v>117</v>
       </c>
@@ -2757,7 +2947,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="65"/>
+      <c r="A84" s="74"/>
       <c r="B84" s="10" t="s">
         <v>118</v>
       </c>
@@ -2769,7 +2959,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="65"/>
+      <c r="A85" s="74"/>
       <c r="B85" s="10" t="s">
         <v>119</v>
       </c>
@@ -2781,7 +2971,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="65"/>
+      <c r="A86" s="74"/>
       <c r="B86" s="10" t="s">
         <v>120</v>
       </c>
@@ -2793,7 +2983,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="65"/>
+      <c r="A87" s="74"/>
       <c r="B87" s="10" t="s">
         <v>121</v>
       </c>
@@ -2805,7 +2995,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="65"/>
+      <c r="A88" s="74"/>
       <c r="B88" s="10" t="s">
         <v>122</v>
       </c>
@@ -2817,7 +3007,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="65"/>
+      <c r="A89" s="74"/>
       <c r="B89" s="10" t="s">
         <v>123</v>
       </c>
@@ -2829,7 +3019,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="65"/>
+      <c r="A90" s="74"/>
       <c r="B90" s="10" t="s">
         <v>124</v>
       </c>
@@ -2841,7 +3031,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="65"/>
+      <c r="A91" s="74"/>
       <c r="B91" s="10" t="s">
         <v>125</v>
       </c>
@@ -2853,7 +3043,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="65"/>
+      <c r="A92" s="74"/>
       <c r="B92" s="10" t="s">
         <v>126</v>
       </c>
@@ -2865,7 +3055,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="66"/>
+      <c r="A93" s="75"/>
       <c r="B93" s="12" t="s">
         <v>49</v>
       </c>
@@ -6344,4 +6534,281 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99807E8C-EE63-4A76-8E1C-D22B4AB455E8}">
+  <dimension ref="A1:R18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="40.7109375" style="1" customWidth="1"/>
+    <col min="6" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="9.140625" style="1"/>
+    <col min="18" max="18" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="89" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+    </row>
+    <row r="2" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="94" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="93"/>
+      <c r="C2" s="79">
+        <v>10</v>
+      </c>
+      <c r="D2" s="84" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" s="80">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="92" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" s="93"/>
+      <c r="C3" s="79">
+        <f>C2*5</f>
+        <v>50</v>
+      </c>
+      <c r="D3" s="84" t="s">
+        <v>254</v>
+      </c>
+      <c r="E3" s="80">
+        <f>C3*E2</f>
+        <v>850000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="92" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" s="93"/>
+      <c r="C4" s="79">
+        <f>SUM(D7:D14)</f>
+        <v>12</v>
+      </c>
+      <c r="D4" s="84" t="s">
+        <v>256</v>
+      </c>
+      <c r="E4" s="95">
+        <f>(E3*C4)-((E3*C4)*0%)</f>
+        <v>10200000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="81"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="83"/>
+      <c r="R5" s="43"/>
+    </row>
+    <row r="6" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="87" t="s">
+        <v>261</v>
+      </c>
+      <c r="B6" s="84" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="84" t="s">
+        <v>257</v>
+      </c>
+      <c r="E6" s="84" t="s">
+        <v>252</v>
+      </c>
+      <c r="M6" s="43"/>
+    </row>
+    <row r="7" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="77">
+        <v>1</v>
+      </c>
+      <c r="B7" s="77" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" s="84" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7" s="85">
+        <v>2</v>
+      </c>
+      <c r="E7" s="86">
+        <f>$E$4*5%</f>
+        <v>510000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="77"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="87" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+    </row>
+    <row r="9" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="90">
+        <v>2</v>
+      </c>
+      <c r="B9" s="90" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" s="91"/>
+      <c r="D9" s="88">
+        <v>2</v>
+      </c>
+      <c r="E9" s="80">
+        <f>$E$4*10%</f>
+        <v>1020000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="84">
+        <v>3</v>
+      </c>
+      <c r="B10" s="84" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="78"/>
+      <c r="D10" s="79">
+        <v>1</v>
+      </c>
+      <c r="E10" s="80">
+        <f>$E$4*10%</f>
+        <v>1020000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="77">
+        <v>4</v>
+      </c>
+      <c r="B11" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="79">
+        <v>1</v>
+      </c>
+      <c r="E11" s="86">
+        <f>$E$4*60%</f>
+        <v>6120000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="77"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" s="79">
+        <v>3</v>
+      </c>
+      <c r="E12" s="85"/>
+    </row>
+    <row r="13" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="77">
+        <v>5</v>
+      </c>
+      <c r="B13" s="77" t="s">
+        <v>238</v>
+      </c>
+      <c r="C13" s="78" t="s">
+        <v>239</v>
+      </c>
+      <c r="D13" s="79">
+        <v>1.5</v>
+      </c>
+      <c r="E13" s="80">
+        <f>$E$4*7.5%</f>
+        <v>765000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="77"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="78" t="s">
+        <v>240</v>
+      </c>
+      <c r="D14" s="79">
+        <v>1.5</v>
+      </c>
+      <c r="E14" s="80">
+        <f>$E$4*7.5%</f>
+        <v>765000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="81"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="83"/>
+    </row>
+    <row r="16" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="92" t="s">
+        <v>262</v>
+      </c>
+      <c r="B16" s="99"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="93"/>
+    </row>
+    <row r="17" spans="1:5" ht="300" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="96" t="s">
+        <v>264</v>
+      </c>
+      <c r="B17" s="97"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="97"/>
+      <c r="E17" s="98"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A13:A14"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.11811023622047245" footer="0.11811023622047245"/>
+  <pageSetup scale="50" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>